<commit_message>
New values for upper and lower bound.
</commit_message>
<xml_diff>
--- a/Settings/datafeeds_settings/RSE_settings.xlsx
+++ b/Settings/datafeeds_settings/RSE_settings.xlsx
@@ -411,7 +411,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,7 +439,7 @@
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -463,10 +463,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -479,10 +479,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C7">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -490,7 +490,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -525,10 +525,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C12">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -536,10 +536,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C13">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -547,7 +547,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C14">
         <v>0.05</v>
@@ -569,7 +569,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C16">
         <v>0.05</v>
@@ -580,7 +580,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="C17">
         <v>0.05</v>
@@ -591,10 +591,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="C18">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -602,10 +602,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C19">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New names for WSA data feeds were tested and function.
</commit_message>
<xml_diff>
--- a/Settings/datafeeds_settings/RSE_settings.xlsx
+++ b/Settings/datafeeds_settings/RSE_settings.xlsx
@@ -51,30 +51,6 @@
     <t>RatioConstraints</t>
   </si>
   <si>
-    <t>WSABOFsteel</t>
-  </si>
-  <si>
-    <t>WSAEAFsteel</t>
-  </si>
-  <si>
-    <t>WSAFlatRolledProducts</t>
-  </si>
-  <si>
-    <t>WSAIngots</t>
-  </si>
-  <si>
-    <t>WSALongRolledProducts</t>
-  </si>
-  <si>
-    <t>WSAOHFsteel</t>
-  </si>
-  <si>
-    <t>WSAPigIron</t>
-  </si>
-  <si>
-    <t>WSASpongeIron</t>
-  </si>
-  <si>
     <t>Minimum</t>
   </si>
   <si>
@@ -82,6 +58,30 @@
   </si>
   <si>
     <t>Item</t>
+  </si>
+  <si>
+    <t>SteelOxygenBlownConverters</t>
+  </si>
+  <si>
+    <t>SteelElectricFurnaces</t>
+  </si>
+  <si>
+    <t>FlatRolledProducts</t>
+  </si>
+  <si>
+    <t>LongRolledProducts</t>
+  </si>
+  <si>
+    <t>Ingots</t>
+  </si>
+  <si>
+    <t>SteelOpenHearthFurnaces</t>
+  </si>
+  <si>
+    <t>PigIron</t>
+  </si>
+  <si>
+    <t>SpongeIron</t>
   </si>
 </sst>
 </file>
@@ -125,9 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -420,18 +421,18 @@
     <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -442,12 +443,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -458,7 +459,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -469,12 +470,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -485,7 +486,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -493,7 +494,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -504,7 +505,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -512,7 +513,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -520,9 +521,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>10</v>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B12">
         <v>0.25</v>
@@ -530,10 +531,11 @@
       <c r="C12">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>11</v>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B13">
         <v>0.25</v>
@@ -541,10 +543,11 @@
       <c r="C13">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>12</v>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B14">
         <v>0.25</v>
@@ -552,10 +555,11 @@
       <c r="C14">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>0.3</v>
@@ -563,10 +567,11 @@
       <c r="C15">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>14</v>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B16">
         <v>0.25</v>
@@ -574,10 +579,11 @@
       <c r="C16">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>0.25</v>
@@ -585,10 +591,11 @@
       <c r="C17">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>0.25</v>
@@ -596,10 +603,11 @@
       <c r="C18">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>0.25</v>
@@ -607,6 +615,7 @@
       <c r="C19">
         <v>0.05</v>
       </c>
+      <c r="F19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New WSA data feeds included, not tested yet.Adapated other feeds.
</commit_message>
<xml_diff>
--- a/Settings/datafeeds_settings/RSE_settings.xlsx
+++ b/Settings/datafeeds_settings/RSE_settings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>BACI</t>
   </si>
@@ -33,9 +33,6 @@
     <t>IRPextraction</t>
   </si>
   <si>
-    <t>IRPextractionHARD</t>
-  </si>
-  <si>
     <t>IRPimports</t>
   </si>
   <si>
@@ -82,6 +79,63 @@
   </si>
   <si>
     <t>SpongeIron</t>
+  </si>
+  <si>
+    <t>HotRolledProducts</t>
+  </si>
+  <si>
+    <t>ContinuouslyCastSteel</t>
+  </si>
+  <si>
+    <t>LiquidSteelForCastings</t>
+  </si>
+  <si>
+    <t>TotalProductionOfCrudeSteel</t>
+  </si>
+  <si>
+    <t>RailwayTrackMaterial</t>
+  </si>
+  <si>
+    <t>HeavySections</t>
+  </si>
+  <si>
+    <t>LightSections</t>
+  </si>
+  <si>
+    <t>ConcreteReinforcingBars</t>
+  </si>
+  <si>
+    <t>HotRolledBarsOtherThanConcreteReinforcingBars</t>
+  </si>
+  <si>
+    <t>WireRod</t>
+  </si>
+  <si>
+    <t>HotRolledPlate</t>
+  </si>
+  <si>
+    <t>HotRolledCoilSheetStrip</t>
+  </si>
+  <si>
+    <t>ElectricalSheetAndStrip</t>
+  </si>
+  <si>
+    <t>TinmillProducts</t>
+  </si>
+  <si>
+    <t>OtherMetalCoatedAndSheetandStrip</t>
+  </si>
+  <si>
+    <t>OtherNonMetalCoatedAndSheetandStrip</t>
+  </si>
+  <si>
+    <t>TubesAndTubeFittings</t>
+  </si>
+  <si>
+    <t>SeamlessTubes</t>
+  </si>
+  <si>
+    <t>WeldedTubes</t>
   </si>
 </sst>
 </file>
@@ -125,10 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -423,13 +479,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -474,16 +530,19 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>0.3</v>
+      </c>
+      <c r="C6">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.3</v>
-      </c>
-      <c r="C7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -491,7 +550,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.2</v>
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -499,10 +561,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
-      </c>
-      <c r="C9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -510,15 +569,18 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>9</v>
+      <c r="A11" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>0.1</v>
+        <v>0.25</v>
+      </c>
+      <c r="C11">
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -546,32 +608,32 @@
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+      <c r="C14">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14">
-        <v>0.25</v>
-      </c>
-      <c r="C14">
-        <v>0.05</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>0.25</v>
+      </c>
+      <c r="C15">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>17</v>
-      </c>
-      <c r="B15">
-        <v>0.3</v>
-      </c>
-      <c r="C15">
-        <v>0.1</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="B16">
         <v>0.25</v>
@@ -606,7 +668,7 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B19">
@@ -616,6 +678,204 @@
         <v>0.05</v>
       </c>
       <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>0.25</v>
+      </c>
+      <c r="C20">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>0.4</v>
+      </c>
+      <c r="C21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>0.2</v>
+      </c>
+      <c r="C22">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>0.25</v>
+      </c>
+      <c r="C23">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>0.25</v>
+      </c>
+      <c r="C24">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>0.25</v>
+      </c>
+      <c r="C25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>0.25</v>
+      </c>
+      <c r="C26">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>0.25</v>
+      </c>
+      <c r="C27">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>0.25</v>
+      </c>
+      <c r="C28">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>0.25</v>
+      </c>
+      <c r="C29">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>0.25</v>
+      </c>
+      <c r="C30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>0.4</v>
+      </c>
+      <c r="C31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>0.4</v>
+      </c>
+      <c r="C32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>0.4</v>
+      </c>
+      <c r="C33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>0.4</v>
+      </c>
+      <c r="C34">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>0.4</v>
+      </c>
+      <c r="C35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>0.4</v>
+      </c>
+      <c r="C36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>0.4</v>
+      </c>
+      <c r="C37">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New China-RoW aggregator added.
</commit_message>
<xml_diff>
--- a/Settings/datafeeds_settings/RSE_settings.xlsx
+++ b/Settings/datafeeds_settings/RSE_settings.xlsx
@@ -468,7 +468,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,10 +493,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>